<commit_message>
Finish orange, implement import script, add translations
</commit_message>
<xml_diff>
--- a/e2x2n-Abyssal_Terrors_Adjustion/translations/translations.xlsx
+++ b/e2x2n-Abyssal_Terrors_Adjustion/translations/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ephemeral\Desktop\BRO\mods-unpacked\e2x2n-Abyssal_Terrors_Adjustion\translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B2AFE8-EA69-4E5F-8AC8-9DAEDFD387DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF835C4-4E2F-4985-AD79-6B1F7ADAB713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>en</t>
   </si>
@@ -52,6 +52,48 @@
   </si>
   <si>
     <t>keys</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>ATA_ITEM_EATEN_ORANGE</t>
+  </si>
+  <si>
+    <t>Eaten Orange</t>
+  </si>
+  <si>
+    <t>吃剩的橘子</t>
+  </si>
+  <si>
+    <t>EFFECT_EATEN_ORANGE</t>
+  </si>
+  <si>
+    <t>The orange has already been eaten.</t>
+  </si>
+  <si>
+    <t>橘子已经被吃完了</t>
+  </si>
+  <si>
+    <t>EFFECT_TEMP_ITEM</t>
+  </si>
+  <si>
+    <t>For the future {0} waves</t>
+  </si>
+  <si>
+    <t>在接下来的{0}个波次中</t>
+  </si>
+  <si>
+    <t>ATA_ITEM_ORANGE_3</t>
+  </si>
+  <si>
+    <t>ATA_ITEM_ORANGE_2</t>
+  </si>
+  <si>
+    <t>ATA_ITEM_ORANGE_1</t>
+  </si>
+  <si>
+    <t>橘子</t>
   </si>
 </sst>
 </file>
@@ -369,15 +411,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -413,6 +457,72 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finish canned food with translation, implement new effect
</commit_message>
<xml_diff>
--- a/e2x2n-Abyssal_Terrors_Adjustion/translations/translations.xlsx
+++ b/e2x2n-Abyssal_Terrors_Adjustion/translations/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ephemeral\Desktop\BRO\mods-unpacked\e2x2n-Abyssal_Terrors_Adjustion\translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF835C4-4E2F-4985-AD79-6B1F7ADAB713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD9BC68-0C81-45BA-A753-0CDAA3783DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>en</t>
   </si>
@@ -81,9 +81,6 @@
     <t>For the future {0} waves</t>
   </si>
   <si>
-    <t>在接下来的{0}个波次中</t>
-  </si>
-  <si>
     <t>ATA_ITEM_ORANGE_3</t>
   </si>
   <si>
@@ -94,6 +91,27 @@
   </si>
   <si>
     <t>橘子</t>
+  </si>
+  <si>
+    <t>在接下来的{0}波敌袭中</t>
+  </si>
+  <si>
+    <t>ATA_ITEM_CANNED_FOOD</t>
+  </si>
+  <si>
+    <t>Canned Food</t>
+  </si>
+  <si>
+    <t>罐装食品</t>
+  </si>
+  <si>
+    <t>EFFECT_GAIN_EVERY_CONSUMABLE</t>
+  </si>
+  <si>
+    <t>Gain 1 {0} when picking up every {1} consumables</t>
+  </si>
+  <si>
+    <t>每当你拾起{0}个消耗品时获得1{1}</t>
   </si>
 </sst>
 </file>
@@ -411,20 +429,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="1" max="1" width="31.453125" customWidth="1"/>
+    <col min="2" max="2" width="43.90625" customWidth="1"/>
+    <col min="3" max="3" width="40.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -435,7 +453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -446,7 +464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -457,40 +475,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -501,7 +519,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -512,7 +530,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -520,7 +538,29 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish powder_keg and rum, add tags for items
</commit_message>
<xml_diff>
--- a/e2x2n-Abyssal_Terrors_Adjustion/translations/translations.xlsx
+++ b/e2x2n-Abyssal_Terrors_Adjustion/translations/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ephemeral\Desktop\BRO\mods-unpacked\e2x2n-Abyssal_Terrors_Adjustion\translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD9BC68-0C81-45BA-A753-0CDAA3783DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391E5522-4B3A-4798-8902-A13C314B9FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>en</t>
   </si>
@@ -112,6 +112,39 @@
   </si>
   <si>
     <t>每当你拾起{0}个消耗品时获得1{1}</t>
+  </si>
+  <si>
+    <t>ATA_ITEM_POWDER_KEG</t>
+  </si>
+  <si>
+    <t>火药桶</t>
+  </si>
+  <si>
+    <t>Powder Keg</t>
+  </si>
+  <si>
+    <t>Rum</t>
+  </si>
+  <si>
+    <t>朗姆酒</t>
+  </si>
+  <si>
+    <t>ATA_ITEM_RUM_5</t>
+  </si>
+  <si>
+    <t>ATA_ITEM_RUM_4</t>
+  </si>
+  <si>
+    <t>ATA_ITEM_RUM_3</t>
+  </si>
+  <si>
+    <t>ATA_ITEM_RUM_2</t>
+  </si>
+  <si>
+    <t>ATA_ITEM_RUM_1</t>
+  </si>
+  <si>
+    <t>ATA_ITEM_RUM_0</t>
   </si>
 </sst>
 </file>
@@ -429,20 +462,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.453125" customWidth="1"/>
-    <col min="2" max="2" width="43.90625" customWidth="1"/>
-    <col min="3" max="3" width="40.54296875" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -453,7 +486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -464,7 +497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -475,7 +508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -486,7 +519,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -497,7 +530,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -508,7 +541,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -519,7 +552,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -530,7 +563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -541,7 +574,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -552,7 +585,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -561,6 +594,83 @@
       </c>
       <c r="C11" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish bow of abyss
</commit_message>
<xml_diff>
--- a/e2x2n-Abyssal_Terrors_Adjustion/translations/translations.xlsx
+++ b/e2x2n-Abyssal_Terrors_Adjustion/translations/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ephemeral\Desktop\BRO\mods-unpacked\e2x2n-Abyssal_Terrors_Adjustion\translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD8137A-CCF3-497A-A149-CD670E4D8C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4461BA7-EF90-4CF2-A1FD-8BEBD41002B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>en</t>
   </si>
@@ -81,15 +81,6 @@
     <t>For the future {0} waves</t>
   </si>
   <si>
-    <t>ATA_ITEM_ORANGE_3</t>
-  </si>
-  <si>
-    <t>ATA_ITEM_ORANGE_2</t>
-  </si>
-  <si>
-    <t>ATA_ITEM_ORANGE_1</t>
-  </si>
-  <si>
     <t>橘子</t>
   </si>
   <si>
@@ -129,24 +120,6 @@
     <t>朗姆酒</t>
   </si>
   <si>
-    <t>ATA_ITEM_RUM_5</t>
-  </si>
-  <si>
-    <t>ATA_ITEM_RUM_4</t>
-  </si>
-  <si>
-    <t>ATA_ITEM_RUM_3</t>
-  </si>
-  <si>
-    <t>ATA_ITEM_RUM_2</t>
-  </si>
-  <si>
-    <t>ATA_ITEM_RUM_1</t>
-  </si>
-  <si>
-    <t>ATA_ITEM_RUM_0</t>
-  </si>
-  <si>
     <t>ATA_ITEM_TOBACCO_PIPE</t>
   </si>
   <si>
@@ -163,6 +136,21 @@
   </si>
   <si>
     <t>航海日志</t>
+  </si>
+  <si>
+    <t>ATA_ITEM_RUM</t>
+  </si>
+  <si>
+    <t>ATA_ITEM_ORANGE</t>
+  </si>
+  <si>
+    <t>ATA_WEAPON_BOW_OF_ABYSS</t>
+  </si>
+  <si>
+    <t>触手弓</t>
+  </si>
+  <si>
+    <t>Tentacle Bow</t>
   </si>
 </sst>
 </file>
@@ -480,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,101 +516,101 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -630,87 +618,21 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
         <v>40</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new weapon set 'horrific', change the set of bow of abyss
</commit_message>
<xml_diff>
--- a/e2x2n-Abyssal_Terrors_Adjustion/translations/translations.xlsx
+++ b/e2x2n-Abyssal_Terrors_Adjustion/translations/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ephemeral\Desktop\BRO\mods-unpacked\e2x2n-Abyssal_Terrors_Adjustion\translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4461BA7-EF90-4CF2-A1FD-8BEBD41002B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31501586-2CA1-4B5B-AD43-5DD8EDD486E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>en</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>Tentacle Bow</t>
+  </si>
+  <si>
+    <t>ATA_WEAPON_CLASS_HORRIFIC</t>
+  </si>
+  <si>
+    <t>Horrific</t>
+  </si>
+  <si>
+    <t>暗渊</t>
   </si>
 </sst>
 </file>
@@ -468,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,6 +644,17 @@
         <v>40</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finish tentacle_gun, modify the horrific set
</commit_message>
<xml_diff>
--- a/e2x2n-Abyssal_Terrors_Adjustion/translations/translations.xlsx
+++ b/e2x2n-Abyssal_Terrors_Adjustion/translations/translations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ephemeral\Desktop\BRO\mods-unpacked\e2x2n-Abyssal_Terrors_Adjustion\translations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ephemeral\Desktop\BRONEW\mods-unpacked\e2x2n-Abyssal_Terrors_Adjustion\translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31501586-2CA1-4B5B-AD43-5DD8EDD486E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EFC1E0-AE80-449A-86FD-A55B35B69304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>en</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>暗渊</t>
+  </si>
+  <si>
+    <t>ATA_WEAPON_TENTACLE_GUN</t>
+  </si>
+  <si>
+    <t>Tentacle Gun</t>
+  </si>
+  <si>
+    <t>触手枪</t>
   </si>
 </sst>
 </file>
@@ -477,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,6 +664,17 @@
         <v>44</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add new stat Disease with icon and color
</commit_message>
<xml_diff>
--- a/e2x2n-Abyssal_Terrors_Adjustion/translations/translations.xlsx
+++ b/e2x2n-Abyssal_Terrors_Adjustion/translations/translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ephemeral\Desktop\BRONEW\mods-unpacked\e2x2n-Abyssal_Terrors_Adjustion\translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EFC1E0-AE80-449A-86FD-A55B35B69304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BD915B-D455-4664-9B71-C2FC39AEEC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>en</t>
   </si>
@@ -169,6 +169,24 @@
   </si>
   <si>
     <t>触手枪</t>
+  </si>
+  <si>
+    <t>ATA_stat_disease</t>
+  </si>
+  <si>
+    <t>Disease</t>
+  </si>
+  <si>
+    <t>疫病</t>
+  </si>
+  <si>
+    <t>INFO_POS_STAT_DISEASE</t>
+  </si>
+  <si>
+    <t>Disease will Disease will reduce your maximum HP, and once your disease level reaches 100, you lose the current game.</t>
+  </si>
+  <si>
+    <t>疾病会削减你的最大生命值，当你的疾病值达到100时，你输掉本局游戏。</t>
   </si>
 </sst>
 </file>
@@ -486,17 +504,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" customWidth="1"/>
+    <col min="2" max="2" width="112.5703125" customWidth="1"/>
+    <col min="3" max="3" width="72.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -675,6 +693,28 @@
         <v>47</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>